<commit_message>
before apply experimental scroll
</commit_message>
<xml_diff>
--- a/resources/works.xlsx
+++ b/resources/works.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ttkmw/beyond-eyesight/workasme/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53D8004A-1C96-2942-81B8-13ADF87DC0DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D74AF0C1-46BA-044F-B6E5-36BCA6BB2708}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-20" yWindow="560" windowWidth="28800" windowHeight="16040" activeTab="1" xr2:uid="{E31C5CC0-24F5-8942-ADB8-59899293243B}"/>
+    <workbookView xWindow="0" yWindow="560" windowWidth="28800" windowHeight="16040" xr2:uid="{E31C5CC0-24F5-8942-ADB8-59899293243B}"/>
   </bookViews>
   <sheets>
     <sheet name="todo list(day)" sheetId="2" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1040" uniqueCount="438">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1106" uniqueCount="464">
   <si>
     <t>F</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -1747,6 +1747,115 @@
   </si>
   <si>
     <t>TaskFinished</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Management Self Section 중 layout</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ttkmwStopped</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>RootLim work out</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>뭘 그렇게 많이 쳐먹냐….</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>코딩 오랜만에 한거치고 좋았는데, 이것저것 먹은게 너무 많음</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>OnGoing,
+TaskFinished</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>TaskStopped,
+TimeTracked</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>make root lim work out</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>IdeaCreated:RootLim:비서가 일정조정 및 외부 만남(회의) 등 정리하게하기. 그리고 한 User당 한 Secretary를 둬야 기록하기 편한듯</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0.6 hour</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>RootSecretaryOff</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>TaskFinished:RootLimSecretary</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>junk sound make beat</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>여기다 뭐쓰는거였지?</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>운동 굿</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>TaskStarted,
+TaskFinished</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>make one beat</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>JunkSoundFocused</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>JunkSoundReady? Or RootLimWashFinished</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MakeAnotherBeatWithFLStudio(JunkSoundMakingBeatFinished)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>TaskStarted,
+TaskFinished,
+TimeTracked</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Timetracked</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>wash body</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>체인지업 슬랙 들어가기</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ETC(DocumentTation?)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Customer</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1805,7 +1914,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1837,6 +1946,9 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="19" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2193,8 +2305,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{6F0613A8-F193-1746-9201-3E95CB31A162}" name="표3" displayName="표3" ref="A3:V59" totalsRowShown="0" dataDxfId="43">
-  <autoFilter ref="A3:V59" xr:uid="{F235149E-6CF9-B843-8E05-1F129098F0AD}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{6F0613A8-F193-1746-9201-3E95CB31A162}" name="표3" displayName="표3" ref="A3:V62" totalsRowShown="0" dataDxfId="43">
+  <autoFilter ref="A3:V62" xr:uid="{F235149E-6CF9-B843-8E05-1F129098F0AD}"/>
   <tableColumns count="22">
     <tableColumn id="1" xr3:uid="{2FEBF9ED-D1F3-CE44-B1BE-684C1DD3520D}" name="Start Date" dataDxfId="42"/>
     <tableColumn id="5" xr3:uid="{FFB9D5D7-A599-E345-B389-F7191FE29828}" name="Start Time" dataDxfId="41"/>
@@ -2591,10 +2703,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AFE457DB-F3F7-A040-8FE3-49840E1A123B}">
-  <dimension ref="A1:S20"/>
+  <dimension ref="A1:S21"/>
   <sheetViews>
-    <sheetView topLeftCell="A8" zoomScale="117" workbookViewId="0">
-      <selection activeCell="P16" sqref="P16"/>
+    <sheetView tabSelected="1" zoomScale="117" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18"/>
@@ -2606,6 +2718,8 @@
     <col min="13" max="13" width="22.140625" customWidth="1"/>
     <col min="14" max="14" width="29.7109375" customWidth="1"/>
     <col min="15" max="15" width="23.28515625" customWidth="1"/>
+    <col min="16" max="16" width="28.140625" customWidth="1"/>
+    <col min="17" max="17" width="23.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19" ht="76">
@@ -2838,7 +2952,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="5" spans="1:19" ht="95">
+    <row r="5" spans="1:19" ht="95" hidden="1">
       <c r="A5" s="8">
         <v>44378</v>
       </c>
@@ -3689,28 +3803,65 @@
         <v>269</v>
       </c>
     </row>
-    <row r="20" spans="1:19">
+    <row r="20" spans="1:19" ht="38" hidden="1">
       <c r="A20" s="4">
         <v>44378</v>
       </c>
-      <c r="B20" s="2"/>
-      <c r="C20" s="2"/>
-      <c r="D20" s="2"/>
-      <c r="E20" s="2"/>
-      <c r="F20" s="2"/>
-      <c r="G20" s="2"/>
-      <c r="H20" s="2"/>
-      <c r="I20" s="2"/>
-      <c r="J20" s="2"/>
-      <c r="K20" s="2"/>
-      <c r="L20" s="2"/>
-      <c r="M20" s="2"/>
-      <c r="N20" s="2"/>
+      <c r="B20" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>338</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>461</v>
+      </c>
+      <c r="F20" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="G20" s="2" t="s">
+        <v>432</v>
+      </c>
+      <c r="H20" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="I20" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="J20" s="2" t="s">
+        <v>434</v>
+      </c>
+      <c r="K20" s="2" t="s">
+        <v>462</v>
+      </c>
+      <c r="L20" s="2" t="s">
+        <v>463</v>
+      </c>
+      <c r="M20" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="N20" s="2" t="s">
+        <v>0</v>
+      </c>
       <c r="O20" s="2"/>
-      <c r="P20" s="9"/>
-      <c r="Q20" s="2"/>
-      <c r="R20" s="2"/>
-      <c r="S20" s="2"/>
+      <c r="P20" s="9" t="s">
+        <v>386</v>
+      </c>
+      <c r="Q20" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="R20" s="2" t="s">
+        <v>272</v>
+      </c>
+      <c r="S20" s="2" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="21" spans="1:19">
+      <c r="F21" s="2"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -3728,10 +3879,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{18853549-B466-0346-BACD-864EAEBAA247}">
-  <dimension ref="A3:V59"/>
+  <dimension ref="A3:V62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B55" zoomScale="91" zoomScaleNormal="223" workbookViewId="0">
-      <selection activeCell="U59" sqref="U59"/>
+    <sheetView topLeftCell="A56" zoomScale="116" zoomScaleNormal="223" workbookViewId="0">
+      <selection activeCell="K61" sqref="K61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18"/>
@@ -3752,7 +3903,7 @@
     <col min="17" max="17" width="71.140625" customWidth="1"/>
     <col min="18" max="18" width="49.5703125" customWidth="1"/>
     <col min="19" max="19" width="46" customWidth="1"/>
-    <col min="20" max="20" width="10.7109375" customWidth="1"/>
+    <col min="20" max="20" width="24.28515625" customWidth="1"/>
     <col min="21" max="21" width="36.7109375" customWidth="1"/>
   </cols>
   <sheetData>
@@ -5640,7 +5791,7 @@
       </c>
       <c r="V42" s="2"/>
     </row>
-    <row r="43" spans="1:22" ht="171">
+    <row r="43" spans="1:22" ht="76">
       <c r="A43" s="4">
         <v>44351</v>
       </c>
@@ -5742,7 +5893,7 @@
       </c>
       <c r="V44" s="2"/>
     </row>
-    <row r="45" spans="1:22" ht="266">
+    <row r="45" spans="1:22" ht="133">
       <c r="A45" s="4">
         <v>44351</v>
       </c>
@@ -6024,7 +6175,7 @@
       <c r="U51" s="2"/>
       <c r="V51" s="2"/>
     </row>
-    <row r="52" spans="1:22" ht="114">
+    <row r="52" spans="1:22" ht="95">
       <c r="A52" s="4">
         <v>44351</v>
       </c>
@@ -6264,7 +6415,7 @@
       </c>
       <c r="V55" s="2"/>
     </row>
-    <row r="56" spans="1:22" ht="171">
+    <row r="56" spans="1:22" ht="76">
       <c r="A56" s="4">
         <v>44351</v>
       </c>
@@ -6448,21 +6599,25 @@
       <c r="S58" s="2"/>
       <c r="T58" s="2"/>
       <c r="U58" s="2" t="s">
-        <v>168</v>
+        <v>443</v>
       </c>
       <c r="V58" s="2" t="s">
         <v>437</v>
       </c>
     </row>
-    <row r="59" spans="1:22" ht="19">
+    <row r="59" spans="1:22" ht="38">
       <c r="A59" s="4">
         <v>44378</v>
       </c>
       <c r="B59" s="10">
         <v>0.79999999999999993</v>
       </c>
-      <c r="C59" s="4"/>
-      <c r="D59" s="10"/>
+      <c r="C59" s="4">
+        <v>44378</v>
+      </c>
+      <c r="D59" s="10">
+        <v>0.9375</v>
+      </c>
       <c r="E59" s="10" t="s">
         <v>164</v>
       </c>
@@ -6478,19 +6633,217 @@
       <c r="I59" s="2" t="s">
         <v>406</v>
       </c>
-      <c r="J59" s="2"/>
-      <c r="K59" s="2"/>
-      <c r="L59" s="2"/>
-      <c r="M59" s="2"/>
-      <c r="N59" s="2"/>
-      <c r="O59" s="2"/>
-      <c r="P59" s="2"/>
-      <c r="Q59" s="2"/>
-      <c r="R59" s="2"/>
-      <c r="S59" s="2"/>
+      <c r="J59" s="2" t="s">
+        <v>438</v>
+      </c>
+      <c r="K59" s="2" t="s">
+        <v>302</v>
+      </c>
+      <c r="L59" s="2" t="s">
+        <v>407</v>
+      </c>
+      <c r="M59" s="2" t="s">
+        <v>439</v>
+      </c>
+      <c r="N59" s="2" t="s">
+        <v>440</v>
+      </c>
+      <c r="O59" s="2">
+        <v>8</v>
+      </c>
+      <c r="P59" s="2" t="s">
+        <v>441</v>
+      </c>
+      <c r="Q59" s="2" t="s">
+        <v>386</v>
+      </c>
+      <c r="R59" s="2" t="s">
+        <v>442</v>
+      </c>
+      <c r="S59" s="2" t="s">
+        <v>386</v>
+      </c>
       <c r="T59" s="2"/>
-      <c r="U59" s="2"/>
-      <c r="V59" s="2"/>
+      <c r="U59" s="2" t="s">
+        <v>444</v>
+      </c>
+      <c r="V59" s="2" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="60" spans="1:22" ht="38">
+      <c r="A60" s="4">
+        <v>44378</v>
+      </c>
+      <c r="B60" s="10">
+        <v>0.9375</v>
+      </c>
+      <c r="C60" s="4">
+        <v>44378</v>
+      </c>
+      <c r="D60" s="10">
+        <v>0.96597222222222223</v>
+      </c>
+      <c r="E60" s="10" t="s">
+        <v>164</v>
+      </c>
+      <c r="F60" s="10" t="s">
+        <v>371</v>
+      </c>
+      <c r="G60" s="2" t="s">
+        <v>445</v>
+      </c>
+      <c r="H60" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="I60" s="2" t="s">
+        <v>406</v>
+      </c>
+      <c r="J60" s="2" t="s">
+        <v>445</v>
+      </c>
+      <c r="K60" s="2" t="s">
+        <v>447</v>
+      </c>
+      <c r="L60" s="2" t="s">
+        <v>448</v>
+      </c>
+      <c r="M60" s="2" t="s">
+        <v>449</v>
+      </c>
+      <c r="N60" s="2" t="s">
+        <v>450</v>
+      </c>
+      <c r="O60" s="2">
+        <v>10</v>
+      </c>
+      <c r="P60" s="2" t="s">
+        <v>451</v>
+      </c>
+      <c r="Q60" s="2" t="s">
+        <v>386</v>
+      </c>
+      <c r="R60" s="2" t="s">
+        <v>452</v>
+      </c>
+      <c r="S60" s="2" t="s">
+        <v>386</v>
+      </c>
+      <c r="T60" t="s">
+        <v>446</v>
+      </c>
+      <c r="U60" s="2" t="s">
+        <v>453</v>
+      </c>
+      <c r="V60" s="2" t="s">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="61" spans="1:22" ht="57">
+      <c r="A61" s="4">
+        <v>44378</v>
+      </c>
+      <c r="B61" s="10">
+        <v>0.9770833333333333</v>
+      </c>
+      <c r="C61" s="4">
+        <v>44379</v>
+      </c>
+      <c r="D61" s="11">
+        <v>7.6388888888888886E-3</v>
+      </c>
+      <c r="E61" s="10" t="s">
+        <v>164</v>
+      </c>
+      <c r="F61" s="10" t="s">
+        <v>105</v>
+      </c>
+      <c r="G61" s="2" t="s">
+        <v>454</v>
+      </c>
+      <c r="H61" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="I61" s="2" t="s">
+        <v>406</v>
+      </c>
+      <c r="J61" s="2" t="s">
+        <v>454</v>
+      </c>
+      <c r="K61" s="2" t="s">
+        <v>447</v>
+      </c>
+      <c r="L61" s="2" t="s">
+        <v>455</v>
+      </c>
+      <c r="M61" s="2" t="s">
+        <v>456</v>
+      </c>
+      <c r="N61" s="2" t="s">
+        <v>457</v>
+      </c>
+      <c r="O61" s="2">
+        <v>8</v>
+      </c>
+      <c r="P61" s="2"/>
+      <c r="Q61" s="2" t="s">
+        <v>386</v>
+      </c>
+      <c r="R61" s="2" t="s">
+        <v>386</v>
+      </c>
+      <c r="S61" s="2" t="s">
+        <v>386</v>
+      </c>
+      <c r="T61" s="2" t="s">
+        <v>386</v>
+      </c>
+      <c r="U61" s="2" t="s">
+        <v>458</v>
+      </c>
+      <c r="V61" s="2" t="s">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="62" spans="1:22" ht="19">
+      <c r="A62" s="4">
+        <v>44379</v>
+      </c>
+      <c r="B62" s="10">
+        <v>0.49583333333333335</v>
+      </c>
+      <c r="C62" s="4">
+        <v>44379</v>
+      </c>
+      <c r="D62" s="2"/>
+      <c r="E62" s="10" t="s">
+        <v>164</v>
+      </c>
+      <c r="F62" s="10" t="s">
+        <v>371</v>
+      </c>
+      <c r="G62" s="2" t="s">
+        <v>460</v>
+      </c>
+      <c r="H62" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="I62" s="2" t="s">
+        <v>406</v>
+      </c>
+      <c r="J62" s="2"/>
+      <c r="K62" s="2"/>
+      <c r="L62" s="2"/>
+      <c r="M62" s="2"/>
+      <c r="N62" s="2"/>
+      <c r="O62" s="2"/>
+      <c r="P62" s="2"/>
+      <c r="Q62" s="2"/>
+      <c r="R62" s="2"/>
+      <c r="S62" s="2"/>
+      <c r="T62" s="2"/>
+      <c r="U62" s="2"/>
+      <c r="V62" s="2"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>

<commit_message>
ing - add row 중
</commit_message>
<xml_diff>
--- a/resources/works.xlsx
+++ b/resources/works.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ttkmw/beyond-eyesight/workasme/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD43959C-DE6F-3342-8666-68DBE93AE697}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA80E522-1CCC-D544-8931-488D5537EC10}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="540" windowWidth="28800" windowHeight="16040" activeTab="1" xr2:uid="{E31C5CC0-24F5-8942-ADB8-59899293243B}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1320" uniqueCount="511">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1341" uniqueCount="517">
   <si>
     <t>F</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -2047,6 +2047,30 @@
   </si>
   <si>
     <t>develop table</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>wash</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1hour</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>필수불가결한일(생활에)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>research useRef</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2.5 hour</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>eat, stretch</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -2164,6 +2188,69 @@
   </cellStyles>
   <dxfs count="66">
     <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -2234,69 +2321,6 @@
     </dxf>
     <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -2514,39 +2538,39 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{6F0613A8-F193-1746-9201-3E95CB31A162}" name="표3" displayName="표3" ref="A5:W89" totalsRowShown="0" dataDxfId="23">
-  <autoFilter ref="A5:W89" xr:uid="{F235149E-6CF9-B843-8E05-1F129098F0AD}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{6F0613A8-F193-1746-9201-3E95CB31A162}" name="표3" displayName="표3" ref="A5:W93" totalsRowShown="0" dataDxfId="44">
+  <autoFilter ref="A5:W93" xr:uid="{F235149E-6CF9-B843-8E05-1F129098F0AD}"/>
   <tableColumns count="23">
-    <tableColumn id="1" xr3:uid="{2FEBF9ED-D1F3-CE44-B1BE-684C1DD3520D}" name="Start Date" dataDxfId="22"/>
-    <tableColumn id="5" xr3:uid="{FFB9D5D7-A599-E345-B389-F7191FE29828}" name="Start Time" dataDxfId="21"/>
-    <tableColumn id="4" xr3:uid="{0F062D0C-5E3B-C84B-8DA7-518F3D7EC1DF}" name="End Date" dataDxfId="20"/>
-    <tableColumn id="6" xr3:uid="{3F982476-7EF2-9F42-8B00-B8ACA81E57B4}" name="End Time" dataDxfId="19"/>
-    <tableColumn id="13" xr3:uid="{1123AB49-7FA4-AB40-BDB1-A8764C6C514D}" name="User Name" dataDxfId="18"/>
-    <tableColumn id="12" xr3:uid="{EB40849B-C48D-744D-83AE-2F5A6F1F5DE6}" name="Character Name" dataDxfId="17"/>
-    <tableColumn id="2" xr3:uid="{08C66D1B-418E-C548-BCFB-FCF68DC7EEB1}" name="Expected Work" dataDxfId="16"/>
-    <tableColumn id="14" xr3:uid="{485A8DB6-6863-C64A-B768-7B52513301E0}" name="Expected Period" dataDxfId="15"/>
-    <tableColumn id="16" xr3:uid="{9481E569-F82D-A442-B453-18A9930BAA66}" name="ExpectedTimeCategory" dataDxfId="14"/>
-    <tableColumn id="3" xr3:uid="{5E1970AB-C596-1E4D-82CE-E33C0232F966}" name="Actual Work" dataDxfId="13"/>
-    <tableColumn id="9" xr3:uid="{745D474B-6A45-D64E-8A7C-7C610774C2B9}" name="Acutal Period" dataDxfId="12"/>
-    <tableColumn id="24" xr3:uid="{5896052E-6D0F-7A43-9144-A18A3CF6BD48}" name="ActualTimeCategory" dataDxfId="11"/>
-    <tableColumn id="18" xr3:uid="{23B4672C-0E6F-A848-A316-34A65EB21736}" name="ContextChange" dataDxfId="10"/>
-    <tableColumn id="20" xr3:uid="{00C950A3-1544-DB46-BD70-6CEC76FF03FE}" name="TriggerdBy" dataDxfId="9"/>
-    <tableColumn id="19" xr3:uid="{F9C48EEF-3DCC-9C48-A81C-F83DAC648C7A}" name="SuccessingWorkOn(Event)" dataDxfId="8"/>
-    <tableColumn id="8" xr3:uid="{FAED4A61-B3D9-9948-9723-E76502CC7320}" name="Self Feedback Number" dataDxfId="7"/>
-    <tableColumn id="23" xr3:uid="{84031E54-5B38-494E-8664-F0D7C2B7E9B8}" name="OrdinaryTask" dataDxfId="6"/>
-    <tableColumn id="22" xr3:uid="{1917C49F-3C4A-1945-9482-740910E4ADCA}" name="ShouldBeRespected(ShowedPerformance/WowPoint)" dataDxfId="5"/>
-    <tableColumn id="7" xr3:uid="{2562DADF-4F43-B64D-9648-CCFDCDCA42B8}" name="Self Feedback Text" dataDxfId="4"/>
-    <tableColumn id="10" xr3:uid="{76E0BAFE-9B5C-9948-BA57-9A5133BBB457}" name="BottleNeck Logs" dataDxfId="3"/>
-    <tableColumn id="15" xr3:uid="{8FA702C1-AAA9-B640-8588-9D6E8E8CA467}" name="UnExpectedAccident" dataDxfId="2"/>
-    <tableColumn id="11" xr3:uid="{1B632BF0-4E92-A944-94CB-E3F92EB9E963}" name="CurrentStatusLog" dataDxfId="1"/>
-    <tableColumn id="21" xr3:uid="{4CE2114E-17E5-8742-A40E-0B671990938E}" name="CurrentState" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{2FEBF9ED-D1F3-CE44-B1BE-684C1DD3520D}" name="Start Date" dataDxfId="43"/>
+    <tableColumn id="5" xr3:uid="{FFB9D5D7-A599-E345-B389-F7191FE29828}" name="Start Time" dataDxfId="42"/>
+    <tableColumn id="4" xr3:uid="{0F062D0C-5E3B-C84B-8DA7-518F3D7EC1DF}" name="End Date" dataDxfId="41"/>
+    <tableColumn id="6" xr3:uid="{3F982476-7EF2-9F42-8B00-B8ACA81E57B4}" name="End Time" dataDxfId="40"/>
+    <tableColumn id="13" xr3:uid="{1123AB49-7FA4-AB40-BDB1-A8764C6C514D}" name="User Name" dataDxfId="39"/>
+    <tableColumn id="12" xr3:uid="{EB40849B-C48D-744D-83AE-2F5A6F1F5DE6}" name="Character Name" dataDxfId="38"/>
+    <tableColumn id="2" xr3:uid="{08C66D1B-418E-C548-BCFB-FCF68DC7EEB1}" name="Expected Work" dataDxfId="37"/>
+    <tableColumn id="14" xr3:uid="{485A8DB6-6863-C64A-B768-7B52513301E0}" name="Expected Period" dataDxfId="36"/>
+    <tableColumn id="16" xr3:uid="{9481E569-F82D-A442-B453-18A9930BAA66}" name="ExpectedTimeCategory" dataDxfId="35"/>
+    <tableColumn id="3" xr3:uid="{5E1970AB-C596-1E4D-82CE-E33C0232F966}" name="Actual Work" dataDxfId="34"/>
+    <tableColumn id="9" xr3:uid="{745D474B-6A45-D64E-8A7C-7C610774C2B9}" name="Acutal Period" dataDxfId="33"/>
+    <tableColumn id="24" xr3:uid="{5896052E-6D0F-7A43-9144-A18A3CF6BD48}" name="ActualTimeCategory" dataDxfId="32"/>
+    <tableColumn id="18" xr3:uid="{23B4672C-0E6F-A848-A316-34A65EB21736}" name="ContextChange" dataDxfId="31"/>
+    <tableColumn id="20" xr3:uid="{00C950A3-1544-DB46-BD70-6CEC76FF03FE}" name="TriggerdBy" dataDxfId="30"/>
+    <tableColumn id="19" xr3:uid="{F9C48EEF-3DCC-9C48-A81C-F83DAC648C7A}" name="SuccessingWorkOn(Event)" dataDxfId="29"/>
+    <tableColumn id="8" xr3:uid="{FAED4A61-B3D9-9948-9723-E76502CC7320}" name="Self Feedback Number" dataDxfId="28"/>
+    <tableColumn id="23" xr3:uid="{84031E54-5B38-494E-8664-F0D7C2B7E9B8}" name="OrdinaryTask" dataDxfId="27"/>
+    <tableColumn id="22" xr3:uid="{1917C49F-3C4A-1945-9482-740910E4ADCA}" name="ShouldBeRespected(ShowedPerformance/WowPoint)" dataDxfId="26"/>
+    <tableColumn id="7" xr3:uid="{2562DADF-4F43-B64D-9648-CCFDCDCA42B8}" name="Self Feedback Text" dataDxfId="25"/>
+    <tableColumn id="10" xr3:uid="{76E0BAFE-9B5C-9948-BA57-9A5133BBB457}" name="BottleNeck Logs" dataDxfId="24"/>
+    <tableColumn id="15" xr3:uid="{8FA702C1-AAA9-B640-8588-9D6E8E8CA467}" name="UnExpectedAccident" dataDxfId="23"/>
+    <tableColumn id="11" xr3:uid="{1B632BF0-4E92-A944-94CB-E3F92EB9E963}" name="CurrentStatusLog" dataDxfId="22"/>
+    <tableColumn id="21" xr3:uid="{4CE2114E-17E5-8742-A40E-0B671990938E}" name="CurrentState" dataDxfId="21"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{8A95934A-4676-184A-B51A-25898AFC5E88}" name="표1" displayName="표1" ref="A1:R16" totalsRowShown="0" headerRowDxfId="44" dataDxfId="43">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{8A95934A-4676-184A-B51A-25898AFC5E88}" name="표1" displayName="표1" ref="A1:R16" totalsRowShown="0" headerRowDxfId="20" dataDxfId="19">
   <autoFilter ref="A1:R16" xr:uid="{34963C48-FACA-F84A-8A57-EB8B000E2FB1}">
     <filterColumn colId="1">
       <filters>
@@ -2561,24 +2585,24 @@
     </filterColumn>
   </autoFilter>
   <tableColumns count="18">
-    <tableColumn id="18" xr3:uid="{214A0061-A58C-6E4C-B71C-3157317845AD}" name="UserName" dataDxfId="42"/>
-    <tableColumn id="17" xr3:uid="{3733CDD9-E263-BB4D-AB2D-4C178F2E5D7B}" name="AccountName" dataDxfId="41"/>
-    <tableColumn id="2" xr3:uid="{2484F67B-9E19-8D41-8346-F07AC4B2E2D7}" name="Field" dataDxfId="40"/>
-    <tableColumn id="3" xr3:uid="{3D7161F5-C479-9341-92D6-2BA890743AEF}" name="Name" dataDxfId="39"/>
-    <tableColumn id="4" xr3:uid="{912B1E27-CDE1-F54C-8899-481BEAD30928}" name="Description" dataDxfId="38"/>
-    <tableColumn id="5" xr3:uid="{E6DA5388-AE76-6845-9467-9E8F3B22483A}" name="Status" dataDxfId="37"/>
-    <tableColumn id="19" xr3:uid="{A55A41FA-67C5-A14D-90CB-902EBBA05A9A}" name="Log" dataDxfId="36"/>
-    <tableColumn id="6" xr3:uid="{8665A432-B8AE-B44D-80A5-AA70E58DA341}" name="Expected(Self) Period" dataDxfId="35"/>
-    <tableColumn id="7" xr3:uid="{04EA4EFC-DB57-584F-9A8A-C4F676B74BC9}" name="Actual Period" dataDxfId="34"/>
-    <tableColumn id="8" xr3:uid="{B2EE9D2A-607D-8447-BA53-336448744472}" name="Start Point" dataDxfId="33"/>
-    <tableColumn id="9" xr3:uid="{63A3887E-38C2-9048-AD89-4CBC0A4EA598}" name="Finish Point" dataDxfId="32"/>
-    <tableColumn id="10" xr3:uid="{3199EEFF-1145-934B-9428-17702C6B1730}" name="Evaluation(At First/At Last) - 첫인상, 끝인상" dataDxfId="31"/>
-    <tableColumn id="11" xr3:uid="{861140E7-F25F-8D44-A9C4-74BBBBF557CB}" name="Difficult Point" dataDxfId="30"/>
-    <tableColumn id="12" xr3:uid="{78CF7B16-7E80-6A4F-B5FD-6C87D2629269}" name="Importance Level of Difficult Point" dataDxfId="29"/>
-    <tableColumn id="13" xr3:uid="{3083314C-2CD9-4D4E-B2B5-9BCE138C72BE}" name="Feedback(Self)" dataDxfId="28"/>
-    <tableColumn id="14" xr3:uid="{C2CED142-8633-B544-A96E-965F00384CAC}" name="Feedback(From coworkers)" dataDxfId="27"/>
-    <tableColumn id="15" xr3:uid="{E01D2F7C-C691-0148-A233-A995530E6E96}" name="What I Learned" dataDxfId="26"/>
-    <tableColumn id="16" xr3:uid="{54B1AF52-E622-104C-8F07-74A82E1F63C7}" name="Reference" dataDxfId="25"/>
+    <tableColumn id="18" xr3:uid="{214A0061-A58C-6E4C-B71C-3157317845AD}" name="UserName" dataDxfId="18"/>
+    <tableColumn id="17" xr3:uid="{3733CDD9-E263-BB4D-AB2D-4C178F2E5D7B}" name="AccountName" dataDxfId="17"/>
+    <tableColumn id="2" xr3:uid="{2484F67B-9E19-8D41-8346-F07AC4B2E2D7}" name="Field" dataDxfId="16"/>
+    <tableColumn id="3" xr3:uid="{3D7161F5-C479-9341-92D6-2BA890743AEF}" name="Name" dataDxfId="15"/>
+    <tableColumn id="4" xr3:uid="{912B1E27-CDE1-F54C-8899-481BEAD30928}" name="Description" dataDxfId="14"/>
+    <tableColumn id="5" xr3:uid="{E6DA5388-AE76-6845-9467-9E8F3B22483A}" name="Status" dataDxfId="13"/>
+    <tableColumn id="19" xr3:uid="{A55A41FA-67C5-A14D-90CB-902EBBA05A9A}" name="Log" dataDxfId="12"/>
+    <tableColumn id="6" xr3:uid="{8665A432-B8AE-B44D-80A5-AA70E58DA341}" name="Expected(Self) Period" dataDxfId="11"/>
+    <tableColumn id="7" xr3:uid="{04EA4EFC-DB57-584F-9A8A-C4F676B74BC9}" name="Actual Period" dataDxfId="10"/>
+    <tableColumn id="8" xr3:uid="{B2EE9D2A-607D-8447-BA53-336448744472}" name="Start Point" dataDxfId="9"/>
+    <tableColumn id="9" xr3:uid="{63A3887E-38C2-9048-AD89-4CBC0A4EA598}" name="Finish Point" dataDxfId="8"/>
+    <tableColumn id="10" xr3:uid="{3199EEFF-1145-934B-9428-17702C6B1730}" name="Evaluation(At First/At Last) - 첫인상, 끝인상" dataDxfId="7"/>
+    <tableColumn id="11" xr3:uid="{861140E7-F25F-8D44-A9C4-74BBBBF557CB}" name="Difficult Point" dataDxfId="6"/>
+    <tableColumn id="12" xr3:uid="{78CF7B16-7E80-6A4F-B5FD-6C87D2629269}" name="Importance Level of Difficult Point" dataDxfId="5"/>
+    <tableColumn id="13" xr3:uid="{3083314C-2CD9-4D4E-B2B5-9BCE138C72BE}" name="Feedback(Self)" dataDxfId="4"/>
+    <tableColumn id="14" xr3:uid="{C2CED142-8633-B544-A96E-965F00384CAC}" name="Feedback(From coworkers)" dataDxfId="3"/>
+    <tableColumn id="15" xr3:uid="{E01D2F7C-C691-0148-A233-A995530E6E96}" name="What I Learned" dataDxfId="2"/>
+    <tableColumn id="16" xr3:uid="{54B1AF52-E622-104C-8F07-74A82E1F63C7}" name="Reference" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2599,7 +2623,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{5BF5D8DA-BB9C-8E4F-9728-B5B3C50983BC}" name="표5" displayName="표5" ref="A1:L17" totalsRowShown="0">
   <autoFilter ref="A1:L17" xr:uid="{8C4E2D83-616C-424E-8DE5-B4AEF9BC6EA6}"/>
   <tableColumns count="12">
-    <tableColumn id="1" xr3:uid="{48754164-EE3D-8042-8351-9E5BF04F3E92}" name="Name(추후 UUID 형식으로 변경 필요)" dataDxfId="24"/>
+    <tableColumn id="1" xr3:uid="{48754164-EE3D-8042-8351-9E5BF04F3E92}" name="Name(추후 UUID 형식으로 변경 필요)" dataDxfId="0"/>
     <tableColumn id="2" xr3:uid="{4271BE0E-3D4C-6149-B2C4-C681DA278899}" name="CharacterName"/>
     <tableColumn id="3" xr3:uid="{3618F7AD-B21D-0641-AFC6-F2E6ABDD3261}" name="UserName(추후 UserName으로 변경 필요)"/>
     <tableColumn id="13" xr3:uid="{0CADD70A-516C-8D49-A872-A367F77ADC07}" name="HighLevelJob"/>
@@ -4143,10 +4167,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{18853549-B466-0346-BACD-864EAEBAA247}">
-  <dimension ref="A3:W90"/>
+  <dimension ref="A3:W93"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H78" zoomScale="116" zoomScaleNormal="223" workbookViewId="0">
-      <selection activeCell="J87" sqref="J87"/>
+    <sheetView tabSelected="1" topLeftCell="G81" zoomScale="150" zoomScaleNormal="223" workbookViewId="0">
+      <selection activeCell="H89" activeCellId="1" sqref="H94 H89"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18"/>
@@ -8444,8 +8468,177 @@
       <c r="V89" s="2"/>
       <c r="W89" s="2"/>
     </row>
-    <row r="90" spans="1:23">
-      <c r="H90" s="2"/>
+    <row r="90" spans="1:23" ht="19">
+      <c r="A90" s="4">
+        <v>44382</v>
+      </c>
+      <c r="B90" s="10">
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="C90" s="4">
+        <v>44382</v>
+      </c>
+      <c r="D90" s="10">
+        <v>0.5</v>
+      </c>
+      <c r="E90" s="10" t="s">
+        <v>164</v>
+      </c>
+      <c r="F90" s="10" t="s">
+        <v>365</v>
+      </c>
+      <c r="G90" s="2" t="s">
+        <v>511</v>
+      </c>
+      <c r="H90" s="2" t="s">
+        <v>512</v>
+      </c>
+      <c r="I90" s="2" t="s">
+        <v>513</v>
+      </c>
+      <c r="J90" s="2" t="s">
+        <v>511</v>
+      </c>
+      <c r="K90" s="2" t="s">
+        <v>512</v>
+      </c>
+      <c r="L90" s="2"/>
+      <c r="M90" s="2"/>
+      <c r="N90" s="2"/>
+      <c r="O90" s="2"/>
+      <c r="P90" s="2"/>
+      <c r="Q90" s="2"/>
+      <c r="R90" s="2"/>
+      <c r="S90" s="2"/>
+      <c r="T90" s="2"/>
+      <c r="U90" s="2"/>
+      <c r="V90" s="2"/>
+      <c r="W90" s="2"/>
+    </row>
+    <row r="91" spans="1:23" ht="19">
+      <c r="A91" s="4">
+        <v>44382</v>
+      </c>
+      <c r="B91" s="10">
+        <v>0.52083333333333337</v>
+      </c>
+      <c r="C91" s="4">
+        <v>44382</v>
+      </c>
+      <c r="D91" s="10">
+        <v>0.60416666666666663</v>
+      </c>
+      <c r="E91" s="10" t="s">
+        <v>164</v>
+      </c>
+      <c r="F91" s="10" t="s">
+        <v>81</v>
+      </c>
+      <c r="G91" s="2" t="s">
+        <v>514</v>
+      </c>
+      <c r="H91" s="2" t="s">
+        <v>515</v>
+      </c>
+      <c r="I91" s="2"/>
+      <c r="J91" s="2"/>
+      <c r="K91" s="2"/>
+      <c r="L91" s="2"/>
+      <c r="M91" s="2"/>
+      <c r="N91" s="2"/>
+      <c r="O91" s="2"/>
+      <c r="P91" s="2"/>
+      <c r="Q91" s="2"/>
+      <c r="R91" s="2"/>
+      <c r="S91" s="2"/>
+      <c r="T91" s="2"/>
+      <c r="U91" s="2"/>
+      <c r="V91" s="2"/>
+      <c r="W91" s="2"/>
+    </row>
+    <row r="92" spans="1:23" ht="19">
+      <c r="A92" s="4">
+        <v>44382</v>
+      </c>
+      <c r="B92" s="10">
+        <v>0.60416666666666663</v>
+      </c>
+      <c r="C92" s="4">
+        <v>44382</v>
+      </c>
+      <c r="D92" s="10">
+        <v>0.625</v>
+      </c>
+      <c r="E92" s="10" t="s">
+        <v>164</v>
+      </c>
+      <c r="F92" s="10" t="s">
+        <v>365</v>
+      </c>
+      <c r="G92" s="2" t="s">
+        <v>516</v>
+      </c>
+      <c r="H92" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="I92" s="2" t="s">
+        <v>513</v>
+      </c>
+      <c r="J92" s="2" t="s">
+        <v>219</v>
+      </c>
+      <c r="K92" s="2"/>
+      <c r="L92" s="2"/>
+      <c r="M92" s="2"/>
+      <c r="N92" s="2"/>
+      <c r="O92" s="2"/>
+      <c r="P92" s="2"/>
+      <c r="Q92" s="2"/>
+      <c r="R92" s="2"/>
+      <c r="S92" s="2"/>
+      <c r="T92" s="2"/>
+      <c r="U92" s="2"/>
+      <c r="V92" s="2"/>
+      <c r="W92" s="2"/>
+    </row>
+    <row r="93" spans="1:23" ht="19">
+      <c r="A93" s="4">
+        <v>44382</v>
+      </c>
+      <c r="B93" s="10">
+        <v>0.62569444444444444</v>
+      </c>
+      <c r="C93" s="4">
+        <v>44382</v>
+      </c>
+      <c r="D93" s="2"/>
+      <c r="E93" s="10" t="s">
+        <v>164</v>
+      </c>
+      <c r="F93" s="10" t="s">
+        <v>81</v>
+      </c>
+      <c r="G93" s="2" t="s">
+        <v>510</v>
+      </c>
+      <c r="H93" s="2" t="s">
+        <v>299</v>
+      </c>
+      <c r="I93" s="2"/>
+      <c r="J93" s="2"/>
+      <c r="K93" s="2"/>
+      <c r="L93" s="2"/>
+      <c r="M93" s="2"/>
+      <c r="N93" s="2"/>
+      <c r="O93" s="2"/>
+      <c r="P93" s="2"/>
+      <c r="Q93" s="2"/>
+      <c r="R93" s="2"/>
+      <c r="S93" s="2"/>
+      <c r="T93" s="2"/>
+      <c r="U93" s="2"/>
+      <c r="V93" s="2"/>
+      <c r="W93" s="2"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>